<commit_message>
set up bicl sim
</commit_message>
<xml_diff>
--- a/test_data2/true_cols.xlsx
+++ b/test_data2/true_cols.xlsx
@@ -379,13 +379,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -396,10 +396,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -413,10 +413,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -430,10 +430,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -450,13 +450,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -467,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -476,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -515,10 +515,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -538,13 +538,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -569,10 +569,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -626,10 +626,10 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -651,10 +651,10 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -674,10 +674,10 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -722,13 +722,13 @@
         <v>0</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -742,10 +742,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -756,10 +756,10 @@
         <v>0</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -770,13 +770,13 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -790,10 +790,10 @@
         <v>0</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -804,13 +804,13 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -861,10 +861,10 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -906,10 +906,10 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -946,13 +946,13 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -960,13 +960,13 @@
         <v>0</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -986,18 +986,18 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B38" t="n">
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B39" t="n">
         <v>0</v>
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1028,13 +1028,13 @@
         <v>0</v>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -1054,12 +1054,12 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B42" t="n">
         <v>0</v>
@@ -1071,12 +1071,12 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B43" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -1093,10 +1093,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -1133,18 +1133,18 @@
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -1153,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B48" t="n">
         <v>0</v>
@@ -1170,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1198,10 +1198,10 @@
         <v>0</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -1218,10 +1218,10 @@
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -1255,18 +1255,18 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -1283,13 +1283,13 @@
         <v>0</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
@@ -1320,21 +1320,21 @@
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
@@ -1351,13 +1351,13 @@
         <v>0</v>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -1368,13 +1368,13 @@
         <v>0</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -1388,13 +1388,13 @@
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1402,13 +1402,13 @@
         <v>0</v>
       </c>
       <c r="B62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -1419,13 +1419,13 @@
         <v>0</v>
       </c>
       <c r="B63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -1507,13 +1507,13 @@
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1572,10 +1572,10 @@
         <v>0</v>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
         <v>0</v>
@@ -1609,18 +1609,18 @@
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
@@ -1632,12 +1632,12 @@
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
@@ -1654,13 +1654,13 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
@@ -1671,10 +1671,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
@@ -1688,10 +1688,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79" t="n">
         <v>0</v>
@@ -1711,10 +1711,10 @@
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -1722,7 +1722,7 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
@@ -1734,15 +1734,15 @@
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" t="n">
         <v>0</v>
@@ -1762,21 +1762,21 @@
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
         <v>0</v>
@@ -1793,10 +1793,10 @@
         <v>0</v>
       </c>
       <c r="B85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
@@ -1810,13 +1810,13 @@
         <v>0</v>
       </c>
       <c r="B86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
         <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
@@ -1836,18 +1836,18 @@
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90" t="n">
         <v>0</v>
@@ -1887,18 +1887,18 @@
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
         <v>0</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
@@ -1938,15 +1938,15 @@
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94" t="n">
         <v>0</v>
@@ -1960,10 +1960,10 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" t="n">
         <v>0</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
@@ -1986,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -1994,10 +1994,10 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97" t="n">
         <v>0</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -2048,13 +2048,13 @@
         <v>0</v>
       </c>
       <c r="B100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" t="n">
         <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
@@ -2074,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -2150,10 +2150,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -2161,13 +2161,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -2218,10 +2218,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -2229,13 +2229,13 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2266,13 +2266,13 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -2306,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -2331,13 +2331,13 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -2348,13 +2348,13 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -2374,10 +2374,10 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -2391,10 +2391,10 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -2416,10 +2416,10 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -2436,13 +2436,13 @@
         <v>0</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -2450,13 +2450,13 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -2467,10 +2467,10 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -2487,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -2510,15 +2510,15 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -2589,10 +2589,10 @@
         <v>0</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -2603,10 +2603,10 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B33" t="n">
         <v>0</v>
@@ -2649,18 +2649,18 @@
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" t="n">
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" t="n">
         <v>0</v>
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -2691,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -2700,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -2708,10 +2708,10 @@
         <v>0</v>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B38" t="n">
         <v>0</v>
@@ -2734,12 +2734,12 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" t="n">
         <v>0</v>
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -2759,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -2768,15 +2768,15 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B42" t="n">
         <v>0</v>
@@ -2799,7 +2799,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2827,10 +2827,10 @@
         <v>0</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" t="n">
         <v>0</v>
@@ -2853,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2861,7 +2861,7 @@
         <v>0</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -2870,12 +2870,12 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -2884,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -2909,13 +2909,13 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B51" t="n">
         <v>0</v>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -3008,10 +3008,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -3025,10 +3025,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -3042,13 +3042,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -3065,13 +3065,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -3079,10 +3079,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -3119,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -3139,12 +3139,12 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -3153,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -3198,13 +3198,13 @@
         <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -3212,13 +3212,13 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -3232,10 +3232,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -3292,7 +3292,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -3314,13 +3314,13 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -3348,10 +3348,10 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -3377,7 +3377,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -3402,13 +3402,13 @@
         <v>0</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -3419,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -3428,18 +3428,18 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" t="n">
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -3467,10 +3467,10 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -3493,18 +3493,18 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -3518,7 +3518,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" t="n">
         <v>0</v>
@@ -3530,7 +3530,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -3538,10 +3538,10 @@
         <v>0</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -3572,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -3592,10 +3592,10 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -3603,10 +3603,10 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -3623,10 +3623,10 @@
         <v>0</v>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -3657,13 +3657,13 @@
         <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -3671,10 +3671,10 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -3691,10 +3691,10 @@
         <v>0</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -3705,10 +3705,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -3739,13 +3739,13 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46" t="n">
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
@@ -3799,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -3824,10 +3824,10 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -3841,10 +3841,10 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -3875,10 +3875,10 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -3892,10 +3892,10 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
@@ -3912,13 +3912,13 @@
         <v>0</v>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -3946,10 +3946,10 @@
         <v>0</v>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
@@ -4028,7 +4028,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
@@ -4037,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
@@ -4057,18 +4057,18 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
@@ -4088,7 +4088,7 @@
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -4116,10 +4116,10 @@
         <v>0</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
@@ -4133,7 +4133,7 @@
         <v>0</v>
       </c>
       <c r="B69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -4142,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -4150,10 +4150,10 @@
         <v>0</v>
       </c>
       <c r="B70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="n">
         <v>0</v>
@@ -4170,10 +4170,10 @@
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -4181,7 +4181,7 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
@@ -4193,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -4201,7 +4201,7 @@
         <v>0</v>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
@@ -4210,7 +4210,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -4221,13 +4221,13 @@
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -4235,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="B75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
@@ -4244,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -4266,10 +4266,10 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77" t="n">
         <v>0</v>
@@ -4283,10 +4283,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
@@ -4317,7 +4317,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
@@ -4326,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -4334,10 +4334,10 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81" t="n">
         <v>0</v>
@@ -4357,13 +4357,13 @@
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -4385,7 +4385,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
@@ -4394,7 +4394,7 @@
         <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -4411,10 +4411,10 @@
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -4422,10 +4422,10 @@
         <v>0</v>
       </c>
       <c r="B86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
@@ -4445,10 +4445,10 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -4470,10 +4470,10 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
@@ -4493,10 +4493,10 @@
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -4530,15 +4530,15 @@
         <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
@@ -4547,7 +4547,7 @@
         <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
@@ -4567,18 +4567,18 @@
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
@@ -4595,10 +4595,10 @@
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -4609,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="B97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97" t="n">
         <v>0</v>
@@ -4618,12 +4618,12 @@
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
@@ -4635,12 +4635,12 @@
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
@@ -4652,7 +4652,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -4666,18 +4666,18 @@
         <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" t="n">
         <v>0</v>
@@ -4691,13 +4691,13 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B102" t="n">
         <v>0</v>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
@@ -4708,13 +4708,13 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B103" t="n">
         <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
@@ -4742,7 +4742,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B105" t="n">
         <v>0</v>
@@ -4751,7 +4751,7 @@
         <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" t="n">
         <v>0</v>
@@ -4765,13 +4765,13 @@
         <v>0</v>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -4782,10 +4782,10 @@
         <v>0</v>
       </c>
       <c r="C107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -4799,18 +4799,18 @@
         <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B109" t="n">
         <v>0</v>
@@ -4819,7 +4819,7 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -4830,7 +4830,7 @@
         <v>0</v>
       </c>
       <c r="B110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C110" t="n">
         <v>0</v>
@@ -4839,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -4904,10 +4904,10 @@
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -4915,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="B115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115" t="n">
         <v>0</v>
@@ -4924,7 +4924,7 @@
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -4932,10 +4932,10 @@
         <v>0</v>
       </c>
       <c r="B116" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
@@ -4949,13 +4949,13 @@
         <v>0</v>
       </c>
       <c r="B117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" t="n">
         <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117" t="n">
         <v>0</v>
@@ -4980,7 +4980,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B119" t="n">
         <v>0</v>
@@ -4992,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -5014,7 +5014,7 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B121" t="n">
         <v>0</v>
@@ -5023,7 +5023,7 @@
         <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121" t="n">
         <v>0</v>
@@ -5031,13 +5031,13 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B122" t="n">
         <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D122" t="n">
         <v>0</v>
@@ -5051,10 +5051,10 @@
         <v>0</v>
       </c>
       <c r="B123" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D123" t="n">
         <v>0</v>
@@ -5068,10 +5068,10 @@
         <v>0</v>
       </c>
       <c r="B124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D124" t="n">
         <v>0</v>
@@ -5082,13 +5082,13 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B125" t="n">
         <v>0</v>
       </c>
       <c r="C125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D125" t="n">
         <v>0</v>
@@ -5099,7 +5099,7 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B126" t="n">
         <v>0</v>
@@ -5111,18 +5111,18 @@
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B127" t="n">
         <v>0</v>
       </c>
       <c r="C127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D127" t="n">
         <v>0</v>
@@ -5139,24 +5139,24 @@
         <v>0</v>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128" t="n">
         <v>0</v>
       </c>
       <c r="E128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B129" t="n">
         <v>0</v>
       </c>
       <c r="C129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D129" t="n">
         <v>0</v>
@@ -5201,10 +5201,10 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C132" t="n">
         <v>0</v>
@@ -5227,10 +5227,10 @@
         <v>0</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -5252,10 +5252,10 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B135" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C135" t="n">
         <v>0</v>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B136" t="n">
         <v>0</v>
@@ -5281,7 +5281,7 @@
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -5289,7 +5289,7 @@
         <v>0</v>
       </c>
       <c r="B137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C137" t="n">
         <v>0</v>
@@ -5298,7 +5298,7 @@
         <v>0</v>
       </c>
       <c r="E137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -5306,10 +5306,10 @@
         <v>0</v>
       </c>
       <c r="B138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
@@ -5323,13 +5323,13 @@
         <v>0</v>
       </c>
       <c r="B139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E139" t="n">
         <v>0</v>
@@ -5354,7 +5354,7 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B141" t="n">
         <v>0</v>
@@ -5366,18 +5366,18 @@
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B142" t="n">
         <v>0</v>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D142" t="n">
         <v>0</v>
@@ -5394,21 +5394,21 @@
         <v>0</v>
       </c>
       <c r="C143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D143" t="n">
         <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C144" t="n">
         <v>0</v>
@@ -5442,13 +5442,13 @@
         <v>0</v>
       </c>
       <c r="B146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C146" t="n">
         <v>0</v>
       </c>
       <c r="D146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E146" t="n">
         <v>0</v>
@@ -5473,7 +5473,7 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B148" t="n">
         <v>0</v>
@@ -5482,7 +5482,7 @@
         <v>0</v>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E148" t="n">
         <v>0</v>
@@ -5490,7 +5490,7 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B149" t="n">
         <v>0</v>
@@ -5502,15 +5502,15 @@
         <v>0</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C150" t="n">
         <v>0</v>
@@ -5527,13 +5527,13 @@
         <v>0</v>
       </c>
       <c r="B151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C151" t="n">
         <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E151" t="n">
         <v>0</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B152" t="n">
         <v>0</v>
@@ -5550,7 +5550,7 @@
         <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E152" t="n">
         <v>0</v>
@@ -5561,10 +5561,10 @@
         <v>0</v>
       </c>
       <c r="B153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D153" t="n">
         <v>0</v>
@@ -5581,10 +5581,10 @@
         <v>0</v>
       </c>
       <c r="C154" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E154" t="n">
         <v>0</v>
@@ -5626,7 +5626,7 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B157" t="n">
         <v>0</v>
@@ -5638,7 +5638,7 @@
         <v>0</v>
       </c>
       <c r="E157" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -5649,10 +5649,10 @@
         <v>0</v>
       </c>
       <c r="C158" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E158" t="n">
         <v>0</v>
@@ -5663,10 +5663,10 @@
         <v>0</v>
       </c>
       <c r="B159" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D159" t="n">
         <v>0</v>
@@ -5677,7 +5677,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B160" t="n">
         <v>0</v>
@@ -5686,7 +5686,7 @@
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E160" t="n">
         <v>0</v>
@@ -5697,10 +5697,10 @@
         <v>0</v>
       </c>
       <c r="B161" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D161" t="n">
         <v>0</v>
@@ -5734,10 +5734,10 @@
         <v>0</v>
       </c>
       <c r="C163" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E163" t="n">
         <v>0</v>
@@ -5751,10 +5751,10 @@
         <v>0</v>
       </c>
       <c r="C164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E164" t="n">
         <v>0</v>
@@ -5762,7 +5762,7 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B165" t="n">
         <v>0</v>
@@ -5771,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E165" t="n">
         <v>0</v>
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="B166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C166" t="n">
         <v>0</v>
@@ -5791,7 +5791,7 @@
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -5833,7 +5833,7 @@
         <v>0</v>
       </c>
       <c r="B169" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C169" t="n">
         <v>0</v>
@@ -5842,12 +5842,12 @@
         <v>0</v>
       </c>
       <c r="E169" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B170" t="n">
         <v>0</v>
@@ -5856,7 +5856,7 @@
         <v>0</v>
       </c>
       <c r="D170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E170" t="n">
         <v>0</v>
@@ -5867,7 +5867,7 @@
         <v>0</v>
       </c>
       <c r="B171" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C171" t="n">
         <v>0</v>
@@ -5876,7 +5876,7 @@
         <v>0</v>
       </c>
       <c r="E171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -5887,10 +5887,10 @@
         <v>0</v>
       </c>
       <c r="C172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E172" t="n">
         <v>0</v>
@@ -5901,13 +5901,13 @@
         <v>0</v>
       </c>
       <c r="B173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C173" t="n">
         <v>0</v>
       </c>
       <c r="D173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E173" t="n">
         <v>0</v>
@@ -5924,10 +5924,10 @@
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -5935,7 +5935,7 @@
         <v>0</v>
       </c>
       <c r="B175" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C175" t="n">
         <v>0</v>
@@ -5944,18 +5944,18 @@
         <v>0</v>
       </c>
       <c r="E175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B176" t="n">
         <v>0</v>
       </c>
       <c r="C176" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D176" t="n">
         <v>0</v>
@@ -5972,10 +5972,10 @@
         <v>0</v>
       </c>
       <c r="C177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E177" t="n">
         <v>0</v>
@@ -5983,13 +5983,13 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B178" t="n">
         <v>0</v>
       </c>
       <c r="C178" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D178" t="n">
         <v>0</v>
@@ -6000,7 +6000,7 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B179" t="n">
         <v>0</v>
@@ -6009,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="D179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E179" t="n">
         <v>0</v>
@@ -6023,24 +6023,24 @@
         <v>0</v>
       </c>
       <c r="C180" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D180" t="n">
         <v>0</v>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B181" t="n">
         <v>0</v>
       </c>
       <c r="C181" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D181" t="n">
         <v>0</v>
@@ -6051,7 +6051,7 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B182" t="n">
         <v>0</v>
@@ -6060,7 +6060,7 @@
         <v>0</v>
       </c>
       <c r="D182" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E182" t="n">
         <v>0</v>
@@ -6068,7 +6068,7 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B183" t="n">
         <v>0</v>
@@ -6080,7 +6080,7 @@
         <v>0</v>
       </c>
       <c r="E183" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -6088,13 +6088,13 @@
         <v>0</v>
       </c>
       <c r="B184" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C184" t="n">
         <v>0</v>
       </c>
       <c r="D184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E184" t="n">
         <v>0</v>
@@ -6111,10 +6111,10 @@
         <v>0</v>
       </c>
       <c r="D185" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -6122,7 +6122,7 @@
         <v>0</v>
       </c>
       <c r="B186" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C186" t="n">
         <v>0</v>
@@ -6131,7 +6131,7 @@
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -6153,7 +6153,7 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B188" t="n">
         <v>0</v>
@@ -6165,15 +6165,15 @@
         <v>0</v>
       </c>
       <c r="E188" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C189" t="n">
         <v>0</v>
@@ -6224,7 +6224,7 @@
         <v>0</v>
       </c>
       <c r="B192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C192" t="n">
         <v>0</v>
@@ -6233,7 +6233,7 @@
         <v>0</v>
       </c>
       <c r="E192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -6241,7 +6241,7 @@
         <v>0</v>
       </c>
       <c r="B193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C193" t="n">
         <v>0</v>
@@ -6250,7 +6250,7 @@
         <v>0</v>
       </c>
       <c r="E193" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -6258,10 +6258,10 @@
         <v>0</v>
       </c>
       <c r="B194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C194" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D194" t="n">
         <v>0</v>
@@ -6281,18 +6281,18 @@
         <v>0</v>
       </c>
       <c r="D195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E195" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C196" t="n">
         <v>0</v>
@@ -6306,7 +6306,7 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B197" t="n">
         <v>0</v>
@@ -6318,18 +6318,18 @@
         <v>0</v>
       </c>
       <c r="E197" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B198" t="n">
         <v>0</v>
       </c>
       <c r="C198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D198" t="n">
         <v>0</v>
@@ -6346,13 +6346,13 @@
         <v>0</v>
       </c>
       <c r="C199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D199" t="n">
         <v>0</v>
       </c>
       <c r="E199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -6360,13 +6360,13 @@
         <v>0</v>
       </c>
       <c r="B200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C200" t="n">
         <v>0</v>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E200" t="n">
         <v>0</v>
@@ -6374,7 +6374,7 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B201" t="n">
         <v>0</v>
@@ -6386,12 +6386,12 @@
         <v>0</v>
       </c>
       <c r="E201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B202" t="n">
         <v>0</v>
@@ -6400,7 +6400,7 @@
         <v>0</v>
       </c>
       <c r="D202" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E202" t="n">
         <v>0</v>
@@ -6417,15 +6417,15 @@
         <v>0</v>
       </c>
       <c r="D203" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E203" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B204" t="n">
         <v>0</v>
@@ -6437,12 +6437,12 @@
         <v>0</v>
       </c>
       <c r="E204" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B205" t="n">
         <v>0</v>
@@ -6454,12 +6454,12 @@
         <v>0</v>
       </c>
       <c r="E205" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B206" t="n">
         <v>0</v>
@@ -6471,7 +6471,7 @@
         <v>0</v>
       </c>
       <c r="E206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -6493,7 +6493,7 @@
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B208" t="n">
         <v>0</v>
@@ -6505,7 +6505,7 @@
         <v>0</v>
       </c>
       <c r="E208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -6519,10 +6519,10 @@
         <v>0</v>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E209" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">
@@ -6530,7 +6530,7 @@
         <v>0</v>
       </c>
       <c r="B210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C210" t="n">
         <v>0</v>
@@ -6539,7 +6539,7 @@
         <v>0</v>
       </c>
       <c r="E210" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211">
@@ -6561,13 +6561,13 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B212" t="n">
         <v>0</v>
       </c>
       <c r="C212" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D212" t="n">
         <v>0</v>
@@ -6578,10 +6578,10 @@
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C213" t="n">
         <v>0</v>
@@ -6595,7 +6595,7 @@
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B214" t="n">
         <v>0</v>
@@ -6607,7 +6607,7 @@
         <v>0</v>
       </c>
       <c r="E214" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -6629,7 +6629,7 @@
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B216" t="n">
         <v>0</v>
@@ -6641,7 +6641,7 @@
         <v>0</v>
       </c>
       <c r="E216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -6652,10 +6652,10 @@
         <v>0</v>
       </c>
       <c r="C217" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E217" t="n">
         <v>0</v>
@@ -6666,7 +6666,7 @@
         <v>0</v>
       </c>
       <c r="B218" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C218" t="n">
         <v>0</v>
@@ -6675,7 +6675,7 @@
         <v>0</v>
       </c>
       <c r="E218" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -6697,10 +6697,10 @@
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B220" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C220" t="n">
         <v>0</v>
@@ -6731,7 +6731,7 @@
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B222" t="n">
         <v>0</v>
@@ -6743,15 +6743,15 @@
         <v>0</v>
       </c>
       <c r="E222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B223" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C223" t="n">
         <v>0</v>
@@ -6768,7 +6768,7 @@
         <v>0</v>
       </c>
       <c r="B224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C224" t="n">
         <v>0</v>
@@ -6777,7 +6777,7 @@
         <v>0</v>
       </c>
       <c r="E224" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225">
@@ -6785,13 +6785,13 @@
         <v>0</v>
       </c>
       <c r="B225" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C225" t="n">
         <v>0</v>
       </c>
       <c r="D225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E225" t="n">
         <v>0</v>
@@ -6819,10 +6819,10 @@
         <v>0</v>
       </c>
       <c r="B227" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C227" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D227" t="n">
         <v>0</v>
@@ -6833,10 +6833,10 @@
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C228" t="n">
         <v>0</v>
@@ -6850,7 +6850,7 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B229" t="n">
         <v>0</v>
@@ -6859,7 +6859,7 @@
         <v>0</v>
       </c>
       <c r="D229" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E229" t="n">
         <v>0</v>
@@ -6867,10 +6867,10 @@
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B230" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C230" t="n">
         <v>0</v>
@@ -6884,10 +6884,10 @@
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C231" t="n">
         <v>0</v>
@@ -6904,13 +6904,13 @@
         <v>0</v>
       </c>
       <c r="B232" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C232" t="n">
         <v>0</v>
       </c>
       <c r="D232" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E232" t="n">
         <v>0</v>
@@ -6918,10 +6918,10 @@
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B233" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C233" t="n">
         <v>0</v>
@@ -6935,13 +6935,13 @@
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B234" t="n">
         <v>0</v>
       </c>
       <c r="C234" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D234" t="n">
         <v>0</v>
@@ -6955,10 +6955,10 @@
         <v>0</v>
       </c>
       <c r="B235" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D235" t="n">
         <v>0</v>
@@ -6986,7 +6986,7 @@
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B237" t="n">
         <v>0</v>
@@ -6995,7 +6995,7 @@
         <v>0</v>
       </c>
       <c r="D237" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E237" t="n">
         <v>0</v>
@@ -7003,13 +7003,13 @@
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B238" t="n">
         <v>0</v>
       </c>
       <c r="C238" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D238" t="n">
         <v>0</v>
@@ -7020,7 +7020,7 @@
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B239" t="n">
         <v>0</v>
@@ -7029,7 +7029,7 @@
         <v>0</v>
       </c>
       <c r="D239" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E239" t="n">
         <v>0</v>
@@ -7037,10 +7037,10 @@
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C240" t="n">
         <v>0</v>
@@ -7057,13 +7057,13 @@
         <v>0</v>
       </c>
       <c r="B241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C241" t="n">
         <v>0</v>
       </c>
       <c r="D241" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E241" t="n">
         <v>0</v>
@@ -7077,10 +7077,10 @@
         <v>0</v>
       </c>
       <c r="C242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D242" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E242" t="n">
         <v>0</v>
@@ -7088,13 +7088,13 @@
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B243" t="n">
         <v>0</v>
       </c>
       <c r="C243" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D243" t="n">
         <v>0</v>
@@ -7142,13 +7142,13 @@
         <v>0</v>
       </c>
       <c r="B246" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C246" t="n">
         <v>0</v>
       </c>
       <c r="D246" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E246" t="n">
         <v>0</v>
@@ -7162,10 +7162,10 @@
         <v>0</v>
       </c>
       <c r="C247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D247" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E247" t="n">
         <v>0</v>
@@ -7173,10 +7173,10 @@
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C248" t="n">
         <v>0</v>
@@ -7207,10 +7207,10 @@
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C250" t="n">
         <v>0</v>

</xml_diff>